<commit_message>
clean-up folder update tasks status
</commit_message>
<xml_diff>
--- a/docs/PM-1 Project Management/PM-1.2 Plans/PM-1.2.1 Project Plan/vms_pm121_implementation_plan_v0.1a.xlsx
+++ b/docs/PM-1 Project Management/PM-1.2 Plans/PM-1.2.1 Project Plan/vms_pm121_implementation_plan_v0.1a.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="167">
   <si>
     <t>No</t>
   </si>
@@ -701,6 +701,9 @@
   </si>
   <si>
     <t>Find code to do upload to table</t>
+  </si>
+  <si>
+    <t>WIP</t>
   </si>
 </sst>
 </file>
@@ -2082,67 +2085,7 @@
     <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="64">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2330,6 +2273,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3905,8 +3878,8 @@
   <dimension ref="A1:N119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4802,7 +4775,7 @@
         <v>40905</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="L25" s="19" t="s">
         <v>86</v>
@@ -5595,7 +5568,7 @@
         <v>3</v>
       </c>
       <c r="G50" s="19" t="s">
-        <v>83</v>
+        <v>166</v>
       </c>
       <c r="H50" s="20">
         <v>40904</v>
@@ -5604,7 +5577,7 @@
         <v>40904</v>
       </c>
       <c r="J50" s="19" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="L50" s="19" t="s">
         <v>86</v>
@@ -5659,7 +5632,7 @@
         <v>5</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>83</v>
+        <v>166</v>
       </c>
       <c r="H52" s="20">
         <v>40906</v>
@@ -5668,7 +5641,7 @@
         <v>40906</v>
       </c>
       <c r="J52" s="19" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="L52" s="19" t="s">
         <v>86</v>
@@ -6830,35 +6803,35 @@
         <v>162</v>
       </c>
     </row>
-    <row r="91" spans="2:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C91" s="19" t="s">
+    <row r="91" spans="2:13" s="21" customFormat="1" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C91" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D91" s="19" t="s">
+      <c r="D91" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="E91" s="19" t="s">
+      <c r="E91" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="F91" s="23">
+      <c r="F91" s="24">
         <v>4</v>
       </c>
-      <c r="G91" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="H91" s="20">
+      <c r="G91" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="H91" s="25">
         <v>40909</v>
       </c>
-      <c r="I91" s="20">
+      <c r="I91" s="25">
         <v>40910</v>
       </c>
-      <c r="J91" s="19" t="s">
+      <c r="J91" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="L91" s="19" t="s">
+      <c r="L91" s="21" t="s">
         <v>86</v>
       </c>
     </row>
@@ -7621,35 +7594,35 @@
         <v>86</v>
       </c>
     </row>
-    <row r="117" spans="2:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="19" t="s">
+    <row r="117" spans="2:12" s="21" customFormat="1" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C117" s="19" t="s">
+      <c r="C117" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="D117" s="19" t="s">
+      <c r="D117" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="E117" s="19" t="s">
+      <c r="E117" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="F117" s="23">
+      <c r="F117" s="24">
         <v>2</v>
       </c>
-      <c r="G117" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="H117" s="20">
+      <c r="G117" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="H117" s="25">
         <v>40909</v>
       </c>
-      <c r="I117" s="20">
+      <c r="I117" s="25">
         <v>40909</v>
       </c>
-      <c r="J117" s="19" t="s">
+      <c r="J117" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="L117" s="19" t="s">
+      <c r="L117" s="21" t="s">
         <v>86</v>
       </c>
     </row>
@@ -7728,228 +7701,229 @@
       <filters>
         <filter val="Done"/>
         <filter val="New"/>
+        <filter val="WIP"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="G1:G71 G75:G82 G84:G87 G93:G1048576">
-    <cfRule type="containsText" dxfId="66" priority="90" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="63" priority="90" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="89" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="62" priority="89" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="88" operator="containsText" text="New">
+    <cfRule type="containsText" dxfId="61" priority="88" operator="containsText" text="New">
       <formula>NOT(ISERROR(SEARCH("New",G1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="84" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="79" operator="containsText" text="''">
+    <cfRule type="containsText" dxfId="59" priority="79" operator="containsText" text="''">
       <formula>NOT(ISERROR(SEARCH("''",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L54 L75:L80 L93:L1048576 L56:L71 L82 L84:L87">
-    <cfRule type="cellIs" dxfId="61" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="80" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="81" operator="containsText" text="New">
+    <cfRule type="containsText" dxfId="57" priority="81" operator="containsText" text="New">
       <formula>NOT(ISERROR(SEARCH("New",L1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="82" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="56" priority="82" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",L1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="83" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="55" priority="83" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G72">
-    <cfRule type="containsText" dxfId="57" priority="70" operator="containsText" text="''">
+    <cfRule type="containsText" dxfId="54" priority="70" operator="containsText" text="''">
       <formula>NOT(ISERROR(SEARCH("''",G72)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="75" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="76" operator="containsText" text="New">
+    <cfRule type="containsText" dxfId="52" priority="76" operator="containsText" text="New">
       <formula>NOT(ISERROR(SEARCH("New",G72)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="77" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="51" priority="77" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",G72)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="78" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="50" priority="78" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G73">
-    <cfRule type="containsText" dxfId="52" priority="61" operator="containsText" text="''">
+    <cfRule type="containsText" dxfId="49" priority="61" operator="containsText" text="''">
       <formula>NOT(ISERROR(SEARCH("''",G73)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="66" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="67" operator="containsText" text="New">
+    <cfRule type="containsText" dxfId="47" priority="67" operator="containsText" text="New">
       <formula>NOT(ISERROR(SEARCH("New",G73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="68" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="46" priority="68" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",G73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="69" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="45" priority="69" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G74">
-    <cfRule type="containsText" dxfId="47" priority="52" operator="containsText" text="''">
+    <cfRule type="containsText" dxfId="44" priority="52" operator="containsText" text="''">
       <formula>NOT(ISERROR(SEARCH("''",G74)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="57" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="58" operator="containsText" text="New">
+    <cfRule type="containsText" dxfId="42" priority="58" operator="containsText" text="New">
       <formula>NOT(ISERROR(SEARCH("New",G74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="59" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="41" priority="59" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",G74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="60" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="40" priority="60" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88:G89">
-    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="''">
+    <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="''">
       <formula>NOT(ISERROR(SEARCH("''",G88)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="48" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="49" operator="containsText" text="New">
+    <cfRule type="containsText" dxfId="37" priority="49" operator="containsText" text="New">
       <formula>NOT(ISERROR(SEARCH("New",G88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="50" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="36" priority="50" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",G88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="51" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="35" priority="51" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G88)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G90">
-    <cfRule type="containsText" dxfId="37" priority="34" operator="containsText" text="''">
+    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="''">
       <formula>NOT(ISERROR(SEARCH("''",G90)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="40" operator="containsText" text="New">
+    <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="New">
       <formula>NOT(ISERROR(SEARCH("New",G90)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="41" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",G90)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="42" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G90)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L88:L90 L81 L72:L74 L55">
-    <cfRule type="containsText" dxfId="32" priority="29" operator="containsText" text="''">
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="''">
       <formula>NOT(ISERROR(SEARCH("''",L55)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="31" operator="containsText" text="New">
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="New">
       <formula>NOT(ISERROR(SEARCH("New",L55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",L55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="25" priority="33" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",L55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I120:I1048576 I1:I118">
-    <cfRule type="timePeriod" dxfId="3" priority="25" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="24" priority="25" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(I1,1)&lt;=6,FLOOR(I1,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="4" priority="2" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="23" priority="2" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(I1,1)&lt;=6,FLOOR(I1,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="5" priority="1" timePeriod="lastMonth">
+    <cfRule type="timePeriod" dxfId="22" priority="1" timePeriod="lastMonth">
       <formula>AND(MONTH(I1)=MONTH(EDATE(TODAY(),0-1)),YEAR(I1)=YEAR(EDATE(TODAY(),0-1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G91:G92">
-    <cfRule type="containsText" dxfId="27" priority="20" operator="containsText" text="''">
+    <cfRule type="containsText" dxfId="21" priority="20" operator="containsText" text="''">
       <formula>NOT(ISERROR(SEARCH("''",G91)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="New">
+    <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="New">
       <formula>NOT(ISERROR(SEARCH("New",G91)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="23" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",G91)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="17" priority="24" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L91:L92">
-    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="''">
+    <cfRule type="containsText" dxfId="16" priority="15" operator="containsText" text="''">
       <formula>NOT(ISERROR(SEARCH("''",L91)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="New">
+    <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="New">
       <formula>NOT(ISERROR(SEARCH("New",L91)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="13" priority="18" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",L91)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="12" priority="19" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",L91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I91:I92">
-    <cfRule type="timePeriod" dxfId="17" priority="14" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="11" priority="14" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(I91,1)&lt;=6,FLOOR(I91,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G83">
-    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="''">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="''">
       <formula>NOT(ISERROR(SEARCH("''",G83)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="New">
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="New">
       <formula>NOT(ISERROR(SEARCH("New",G83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",G83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="6" priority="13" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",G83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L83">
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="''">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="''">
       <formula>NOT(ISERROR(SEARCH("''",L83)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="New">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="New">
       <formula>NOT(ISERROR(SEARCH("New",L83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",L83)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",L83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I83">
-    <cfRule type="timePeriod" dxfId="6" priority="3" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="0" priority="3" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(I83,1)&lt;=6,FLOOR(I83,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>